<commit_message>
Description: Updated requirement specifications. Bug ID: NA Reviewed By: self
</commit_message>
<xml_diff>
--- a/technical/requirement/auto-service-centre/service-center-demo_v1.0.xlsx
+++ b/technical/requirement/auto-service-centre/service-center-demo_v1.0.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="102">
   <si>
     <t>Following links will be displayed</t>
   </si>
@@ -62,36 +62,12 @@
     <t>No changes required</t>
   </si>
   <si>
-    <t>Need to create this page in the product</t>
-  </si>
-  <si>
-    <t>Need to remove, chart and action</t>
-  </si>
-  <si>
     <t>Data grid columns</t>
   </si>
   <si>
-    <t>Ward</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
-    <t>Remove Action</t>
-  </si>
-  <si>
-    <t>General Ward</t>
-  </si>
-  <si>
-    <t>Private Room</t>
-  </si>
-  <si>
-    <t>Semi Private</t>
-  </si>
-  <si>
     <t>ICU</t>
   </si>
   <si>
@@ -312,6 +288,42 @@
   </si>
   <si>
     <t xml:space="preserve">Job Create </t>
+  </si>
+  <si>
+    <t>Filter</t>
+  </si>
+  <si>
+    <t>Vehicle No</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Service Date</t>
+  </si>
+  <si>
+    <t>Today</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Select</t>
+  </si>
+  <si>
+    <t>Similar to graph above the datagrid</t>
+  </si>
+  <si>
+    <t>In time</t>
+  </si>
+  <si>
+    <t>Out Time</t>
+  </si>
+  <si>
+    <t>Token</t>
+  </si>
+  <si>
+    <t>Action</t>
   </si>
 </sst>
 </file>
@@ -708,10 +720,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:I82"/>
+  <dimension ref="B3:I86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="D54" sqref="D54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +765,7 @@
         <v>4</v>
       </c>
       <c r="D7" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.25">
@@ -774,7 +786,7 @@
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>31</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.25">
@@ -787,16 +799,16 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D13" t="s">
         <v>11</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="F13" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.25">
@@ -811,30 +823,30 @@
     </row>
     <row r="17" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C17" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
     </row>
     <row r="18" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C18" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="F18" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="G18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="H18" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="I18" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="19" spans="3:9" x14ac:dyDescent="0.25">
@@ -862,165 +874,165 @@
     </row>
     <row r="21" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C21" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
     </row>
     <row r="22" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C22" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
     </row>
     <row r="23" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="D23" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C24" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C25" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D25" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D27" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E27" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F27" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G27" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H27" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I27" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C28" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D28" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" t="s">
+        <v>82</v>
+      </c>
+      <c r="F28" t="s">
         <v>89</v>
       </c>
-      <c r="E28" t="s">
-        <v>90</v>
-      </c>
-      <c r="F28" t="s">
-        <v>97</v>
-      </c>
       <c r="G28" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H28" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="30" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C30" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="31" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C31" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="D31" t="s">
+        <v>81</v>
+      </c>
+      <c r="E31" t="s">
+        <v>82</v>
+      </c>
+      <c r="F31" t="s">
         <v>89</v>
       </c>
-      <c r="E31" t="s">
-        <v>90</v>
-      </c>
-      <c r="F31" t="s">
-        <v>97</v>
-      </c>
       <c r="G31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="H31" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C33" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="E33" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="F33" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="G33" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="H33" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="I33" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="34" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C36" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
     </row>
     <row r="37" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C37" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="40" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C40" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="41" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C41" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C42" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="43" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C43" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
     </row>
     <row r="45" spans="2:9" x14ac:dyDescent="0.25">
@@ -1033,222 +1045,235 @@
     </row>
     <row r="46" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
-        <v>57</v>
+        <v>49</v>
+      </c>
+      <c r="C46" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="47" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C47" t="s">
-        <v>14</v>
+        <v>91</v>
       </c>
     </row>
     <row r="48" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C48" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C49" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C51" t="s">
+        <v>93</v>
+      </c>
+      <c r="D51" t="s">
+        <v>94</v>
+      </c>
+      <c r="E51" t="s">
+        <v>95</v>
+      </c>
+      <c r="F51" t="s">
+        <v>96</v>
+      </c>
+      <c r="G51" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="53" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C53" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D54" t="s">
+        <v>93</v>
+      </c>
+      <c r="E54" t="s">
+        <v>98</v>
+      </c>
+      <c r="F54" t="s">
+        <v>99</v>
+      </c>
+      <c r="G54" t="s">
+        <v>100</v>
+      </c>
+      <c r="H54" t="s">
+        <v>92</v>
+      </c>
+      <c r="I54" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="57" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="E57" t="s">
         <v>16</v>
       </c>
-      <c r="D49" t="s">
+    </row>
+    <row r="58" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
         <v>17</v>
       </c>
-      <c r="E49" t="s">
+      <c r="C58" t="s">
+        <v>14</v>
+      </c>
+      <c r="D58" t="s">
         <v>18</v>
       </c>
-      <c r="F49" t="s">
+      <c r="E58" t="s">
         <v>19</v>
       </c>
-      <c r="G49" t="s">
+    </row>
+    <row r="60" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="C60" t="s">
+        <v>20</v>
+      </c>
+      <c r="D60" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>9</v>
+      </c>
+      <c r="C62" t="s">
+        <v>22</v>
+      </c>
+      <c r="D62" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="64" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
         <v>5</v>
       </c>
-      <c r="H49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
+      <c r="C64" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+      <c r="D64" t="s">
+        <v>18</v>
+      </c>
+      <c r="E64" t="s">
+        <v>26</v>
+      </c>
+      <c r="F64" t="s">
+        <v>28</v>
+      </c>
+      <c r="G64" t="s">
+        <v>27</v>
+      </c>
+      <c r="H64" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H65" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="66" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="H66" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="67" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C67" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="68" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C68" t="s">
+        <v>38</v>
+      </c>
+      <c r="D68" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="69" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="70" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C70" t="s">
         <v>25</v>
       </c>
-      <c r="C54" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" t="s">
+    </row>
+    <row r="71" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C71" t="s">
         <v>26</v>
       </c>
-      <c r="E54" t="s">
+    </row>
+    <row r="72" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C72" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="73" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C73" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="74" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C74" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C56" t="s">
-        <v>28</v>
-      </c>
-      <c r="D56" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
-        <v>9</v>
-      </c>
-      <c r="C58" t="s">
+    <row r="75" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C75" t="s">
         <v>30</v>
       </c>
-      <c r="D58" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>32</v>
-      </c>
-      <c r="D60" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" t="s">
-        <v>34</v>
-      </c>
-      <c r="F60" t="s">
+    </row>
+    <row r="76" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C76" t="s">
         <v>36</v>
       </c>
-      <c r="G60" t="s">
-        <v>35</v>
-      </c>
-      <c r="H60" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H61" t="s">
+    </row>
+    <row r="77" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C77" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="79" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C79" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="H62" t="s">
+      <c r="D79" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C63" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C64" t="s">
-        <v>46</v>
-      </c>
-      <c r="D64" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="65" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C65" t="s">
+    <row r="80" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C80" t="s">
         <v>42</v>
-      </c>
-    </row>
-    <row r="66" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C66" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="67" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C67" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="68" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C68" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="69" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C69" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="70" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C70" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="71" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C71" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="72" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C72" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="73" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C73" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="75" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C75" t="s">
-        <v>48</v>
-      </c>
-      <c r="D75" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="76" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C76" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="77" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C77" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="78" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C78" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="79" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C79" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="81" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C81" t="s">
-        <v>54</v>
-      </c>
-      <c r="D81" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="82" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C82" t="s">
-        <v>56</v>
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C83" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="85" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C85" t="s">
+        <v>46</v>
+      </c>
+      <c r="D85" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="86" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C86" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>